<commit_message>
Primeros avances Creación de las url, vistas, temlates y estilos
</commit_message>
<xml_diff>
--- a/Lista de tareas pendientes API.xlsx
+++ b/Lista de tareas pendientes API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B97FB4A-5D5E-4A0E-B8D4-1A8ED2EFD0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AD17D9-CF08-4CE1-ADEE-D3BD8271D30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -77,10 +77,19 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Puedo hacerlo rápido con ChatGPT</t>
+    <t xml:space="preserve"> Lista de tareas pendientes proyecto APIs</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lista de tareas pendientes proyecto APIs</t>
+    <t>En progreso</t>
+  </si>
+  <si>
+    <t>Esá bastante avanzado</t>
+  </si>
+  <si>
+    <t>Resta hacer bien el diccionario de contexto, para que traiga las plataformas asociadas al nombre</t>
+  </si>
+  <si>
+    <t>Puede ser utilizando el mismo diccionario del JSON</t>
   </si>
 </sst>
 </file>
@@ -774,7 +783,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -892,6 +901,9 @@
     </xf>
     <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1336,10 +1348,10 @@
       <xdr:rowOff>236220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3116580</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1423737</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1354,8 +1366,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1280160" y="1074420"/>
-          <a:ext cx="9509760" cy="358140"/>
+          <a:off x="1278155" y="1078431"/>
+          <a:ext cx="11355003" cy="515753"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1396,9 +1408,40 @@
           </a:r>
           <a:r>
             <a:rPr lang="es-AR" sz="1200" b="1" baseline="0"/>
-            <a:t> simple.</a:t>
+            <a:t> simple.-- </a:t>
           </a:r>
-          <a:endParaRPr lang="es-AR" sz="1200" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>--</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> HAY QUE TENER CUIDADO CON LA CANTIDAD DE API CALSS QUE HAGO, HAY UN LÍMITE DIARIO. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>--</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1200" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1661,7 +1704,7 @@
   <dimension ref="A1:XFA23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
@@ -1686,7 +1729,7 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="11"/>
@@ -1749,7 +1792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="6" customFormat="1" ht="34.200000000000003" customHeight="1">
+    <row r="6" spans="1:14" s="6" customFormat="1" ht="51" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="15" t="s">
         <v>9</v>
@@ -1771,7 +1814,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="40.200000000000003" customHeight="1">
+    <row r="7" spans="1:14" ht="75">
       <c r="A7" s="40" t="s">
         <v>1</v>
       </c>
@@ -1781,14 +1824,20 @@
       <c r="C7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="F7" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" ht="37.200000000000003" customHeight="1">
+    <row r="8" spans="1:14" ht="64.2" customHeight="1">
       <c r="A8" s="40"/>
       <c r="B8" s="18" t="s">
         <v>13</v>
@@ -1796,9 +1845,11 @@
       <c r="C8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28"/>

</xml_diff>

<commit_message>
Terminada la función principal y el template
</commit_message>
<xml_diff>
--- a/Lista de tareas pendientes API.xlsx
+++ b/Lista de tareas pendientes API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AD17D9-CF08-4CE1-ADEE-D3BD8271D30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4047F8-CA0D-44F9-BC22-9BD30324389A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -80,16 +80,19 @@
     <t xml:space="preserve"> Lista de tareas pendientes proyecto APIs</t>
   </si>
   <si>
-    <t>En progreso</t>
-  </si>
-  <si>
-    <t>Esá bastante avanzado</t>
-  </si>
-  <si>
     <t>Resta hacer bien el diccionario de contexto, para que traiga las plataformas asociadas al nombre</t>
   </si>
   <si>
     <t>Puede ser utilizando el mismo diccionario del JSON</t>
+  </si>
+  <si>
+    <t>Está bastante avanzado</t>
+  </si>
+  <si>
+    <t>Crear la segunda parte con la consulta de los datos de las pelis</t>
+  </si>
+  <si>
+    <t>Probablemente se pueda hacer directamente con una API call similar, porque trae mucha más información, hasta imágenes</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -901,9 +904,6 @@
     </xf>
     <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1703,8 +1703,8 @@
   </sheetPr>
   <dimension ref="A1:XFA23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
@@ -1824,17 +1824,17 @@
       <c r="C7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>16</v>
+      <c r="D7" s="20">
+        <v>1</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>19</v>
+      <c r="F7" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="64.2" customHeight="1">
@@ -1845,21 +1845,27 @@
       <c r="C8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>16</v>
+      <c r="D8" s="20">
+        <v>1</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:14" ht="50.4" customHeight="1">
       <c r="A9" s="40"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="D9" s="36"/>
-      <c r="E9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="F9" s="24"/>
       <c r="G9" s="34"/>
     </row>
@@ -2091,21 +2097,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2317,19 +2323,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se agregaron los ratings y las imágenes
</commit_message>
<xml_diff>
--- a/Lista de tareas pendientes API.xlsx
+++ b/Lista de tareas pendientes API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4047F8-CA0D-44F9-BC22-9BD30324389A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5817E6-B7AD-48E6-B883-9E1D4CAB94DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Probablemente se pueda hacer directamente con una API call similar, porque trae mucha más información, hasta imágenes</t>
+  </si>
+  <si>
+    <t>Mejorar el diseño</t>
+  </si>
+  <si>
+    <t>Ponerlo Online</t>
   </si>
 </sst>
 </file>
@@ -786,7 +792,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -904,6 +910,9 @@
     </xf>
     <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1704,7 +1713,7 @@
   <dimension ref="A1:XFA23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
@@ -1856,30 +1865,40 @@
     </row>
     <row r="9" spans="1:14" ht="50.4" customHeight="1">
       <c r="A9" s="40"/>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="42" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="36">
+        <v>1</v>
+      </c>
       <c r="E9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="34"/>
     </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+    <row r="10" spans="1:14" ht="49.8" customHeight="1">
+      <c r="B10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="D10" s="37"/>
       <c r="E10" s="15"/>
       <c r="F10" s="27"/>
       <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:14" ht="105" customHeight="1">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="D11" s="36"/>
       <c r="E11" s="15"/>
       <c r="F11" s="28"/>
@@ -2097,21 +2116,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2323,19 +2342,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Despliegue en fly.io y video para GitHub
</commit_message>
<xml_diff>
--- a/Lista de tareas pendientes API.xlsx
+++ b/Lista de tareas pendientes API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5817E6-B7AD-48E6-B883-9E1D4CAB94DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0984193-ED9A-42BB-8124-5F6A767916F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Ponerlo Online</t>
+  </si>
+  <si>
+    <t>Hacer los gifs y poner el link</t>
+  </si>
+  <si>
+    <t>Hacer la página de error.</t>
+  </si>
+  <si>
+    <t>Terminar el readme del proyecto y el general</t>
+  </si>
+  <si>
+    <t>HAY QUE CONFIGURAR EL 'DIRS' EN SETTINGS PARA PONER LOS TEMPLATES DE ERROR ONLINE</t>
   </si>
 </sst>
 </file>
@@ -115,7 +127,7 @@
     <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="169" formatCode="&quot;Completado&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14996795556505021"/>
@@ -417,6 +429,12 @@
       <name val="Lucida Sans"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1" tint="0.14996795556505021"/>
+      <name val="Calibri"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -792,7 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -911,8 +929,14 @@
     <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1712,8 +1736,8 @@
   </sheetPr>
   <dimension ref="A1:XFA23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
@@ -1865,7 +1889,7 @@
     </row>
     <row r="9" spans="1:14" ht="50.4" customHeight="1">
       <c r="A9" s="40"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -1887,7 +1911,9 @@
       <c r="C10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="37">
+        <v>1</v>
+      </c>
       <c r="E10" s="15"/>
       <c r="F10" s="27"/>
       <c r="G10" s="22"/>
@@ -1897,7 +1923,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="15"/>
@@ -1905,18 +1931,30 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:14" ht="49.8" customHeight="1">
-      <c r="B12" s="25"/>
-      <c r="C12" s="19"/>
+      <c r="B12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="D12" s="21"/>
-      <c r="E12" s="24"/>
+      <c r="E12" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="F12" s="31"/>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:14" ht="17.399999999999999">
-      <c r="B13" s="25"/>
-      <c r="C13" s="29"/>
+    <row r="13" spans="1:14" ht="54">
+      <c r="B13" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>14</v>
+      </c>
       <c r="D13" s="39"/>
-      <c r="E13" s="30"/>
+      <c r="E13" s="42" t="s">
+        <v>26</v>
+      </c>
       <c r="F13" s="28"/>
       <c r="G13" s="22"/>
     </row>
@@ -2116,21 +2154,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2342,19 +2380,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>